<commit_message>
Se implementan pow y prog dinamica digamos, mejorada nose que poner
</commit_message>
<xml_diff>
--- a/Métricas Polinomio.xlsx
+++ b/Métricas Polinomio.xlsx
@@ -846,23 +846,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -873,23 +862,44 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="7" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -899,14 +909,32 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -917,43 +945,35 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="7" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -1198,10 +1218,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.3333333333333332E-3</c:v>
+                  <c:v>1.0416666666666668E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.2222222222222476E-2</c:v>
+                  <c:v>2.6388888888889017E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1591,7 +1611,7 @@
   <dimension ref="A1:P68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -1606,21 +1626,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="93"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
-      <c r="M1" s="94"/>
-      <c r="N1" s="94"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
     </row>
     <row r="2" spans="1:16" s="10" customFormat="1" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="60"/>
@@ -1639,12 +1659,12 @@
     </row>
     <row r="3" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="70"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="66"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -1725,12 +1745,12 @@
     </row>
     <row r="7" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="70"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="66"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
@@ -1756,15 +1776,15 @@
       <c r="E8" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="66"/>
-      <c r="N8" s="66"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="67"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="67"/>
+      <c r="N8" s="67"/>
       <c r="O8" s="14"/>
       <c r="P8" s="18"/>
     </row>
@@ -1779,15 +1799,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C9),ISBLANK(D9)),"Completar",IF(D9&gt;=C9,D9-C9,"Error")),"Error")</f>
         <v>Completar</v>
       </c>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="67"/>
-      <c r="L9" s="67"/>
-      <c r="M9" s="67"/>
-      <c r="N9" s="67"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="68"/>
+      <c r="J9" s="68"/>
+      <c r="K9" s="68"/>
+      <c r="L9" s="68"/>
+      <c r="M9" s="68"/>
+      <c r="N9" s="68"/>
       <c r="O9" s="19"/>
       <c r="P9" s="22"/>
     </row>
@@ -1811,12 +1831,12 @@
     </row>
     <row r="11" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="70"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="66"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
@@ -1842,15 +1862,15 @@
       <c r="E12" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="66"/>
-      <c r="J12" s="66"/>
-      <c r="K12" s="66"/>
-      <c r="L12" s="66"/>
-      <c r="M12" s="66"/>
-      <c r="N12" s="66"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="67"/>
+      <c r="N12" s="67"/>
       <c r="O12" s="14"/>
       <c r="P12" s="18"/>
     </row>
@@ -1865,15 +1885,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C13),ISBLANK(D13)),"Completar",IF(D13&gt;=C13,D13-C13,"Error")),"Error")</f>
         <v>Completar</v>
       </c>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="67"/>
-      <c r="L13" s="67"/>
-      <c r="M13" s="67"/>
-      <c r="N13" s="67"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="68"/>
+      <c r="M13" s="68"/>
+      <c r="N13" s="68"/>
       <c r="O13" s="19"/>
       <c r="P13" s="22"/>
     </row>
@@ -1897,50 +1917,50 @@
     </row>
     <row r="15" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
-      <c r="B15" s="68" t="s">
+      <c r="B15" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="69"/>
-      <c r="H15" s="69"/>
-      <c r="I15" s="69"/>
-      <c r="J15" s="69"/>
-      <c r="K15" s="69"/>
-      <c r="L15" s="69"/>
-      <c r="M15" s="69"/>
-      <c r="N15" s="70"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
+      <c r="K15" s="65"/>
+      <c r="L15" s="65"/>
+      <c r="M15" s="65"/>
+      <c r="N15" s="66"/>
       <c r="O15" s="11"/>
     </row>
     <row r="16" spans="1:16" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
-      <c r="B16" s="89" t="s">
+      <c r="B16" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="75" t="s">
+      <c r="C16" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="75"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="62" t="s">
+      <c r="D16" s="87"/>
+      <c r="E16" s="88"/>
+      <c r="F16" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="63"/>
-      <c r="H16" s="64" t="s">
+      <c r="G16" s="90"/>
+      <c r="H16" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="75"/>
-      <c r="J16" s="76"/>
-      <c r="K16" s="62" t="s">
+      <c r="I16" s="87"/>
+      <c r="J16" s="88"/>
+      <c r="K16" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="L16" s="63"/>
-      <c r="M16" s="64" t="s">
+      <c r="L16" s="90"/>
+      <c r="M16" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="N16" s="65" t="s">
+      <c r="N16" s="94" t="s">
         <v>2</v>
       </c>
       <c r="O16" s="14"/>
@@ -1948,10 +1968,10 @@
     </row>
     <row r="17" spans="1:16" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
-      <c r="B17" s="89"/>
-      <c r="C17" s="75"/>
-      <c r="D17" s="75"/>
-      <c r="E17" s="76"/>
+      <c r="B17" s="76"/>
+      <c r="C17" s="87"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="88"/>
       <c r="F17" s="39" t="s">
         <v>12</v>
       </c>
@@ -1973,8 +1993,8 @@
       <c r="L17" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="M17" s="64"/>
-      <c r="N17" s="65"/>
+      <c r="M17" s="86"/>
+      <c r="N17" s="94"/>
       <c r="O17" s="14"/>
       <c r="P17" s="18"/>
     </row>
@@ -1984,11 +2004,11 @@
         <f>ROW($B18)-16</f>
         <v>2</v>
       </c>
-      <c r="C18" s="77" t="s">
+      <c r="C18" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="77"/>
-      <c r="E18" s="78"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="81"/>
       <c r="F18" s="3">
         <v>25</v>
       </c>
@@ -2027,11 +2047,11 @@
         <f t="shared" ref="B19:B25" si="0">ROW($B19)-16</f>
         <v>3</v>
       </c>
-      <c r="C19" s="77" t="s">
+      <c r="C19" s="80" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="77"/>
-      <c r="E19" s="78"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="81"/>
       <c r="F19" s="3">
         <v>15</v>
       </c>
@@ -2045,7 +2065,7 @@
         <v>0.73055555555555562</v>
       </c>
       <c r="J19" s="53">
-        <f t="shared" ref="J19:J23" si="1">IFERROR(IF(OR(ISBLANK(H19),ISBLANK(I19)),"",IF(I19&gt;=H19,I19-H19,"Error")),"Error")</f>
+        <f t="shared" ref="J19:J24" si="1">IFERROR(IF(OR(ISBLANK(H19),ISBLANK(I19)),"",IF(I19&gt;=H19,I19-H19,"Error")),"Error")</f>
         <v>3.4722222222223209E-3</v>
       </c>
       <c r="K19" s="7">
@@ -2070,11 +2090,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C20" s="77" t="s">
+      <c r="C20" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="77"/>
-      <c r="E20" s="78"/>
+      <c r="D20" s="80"/>
+      <c r="E20" s="81"/>
       <c r="F20" s="3">
         <v>20</v>
       </c>
@@ -2113,11 +2133,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C21" s="77" t="s">
+      <c r="C21" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="77"/>
-      <c r="E21" s="78"/>
+      <c r="D21" s="80"/>
+      <c r="E21" s="81"/>
       <c r="F21" s="3">
         <v>20</v>
       </c>
@@ -2156,25 +2176,39 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C22" s="77" t="s">
+      <c r="C22" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="77"/>
-      <c r="E22" s="78"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="53" t="str">
+      <c r="D22" s="80"/>
+      <c r="E22" s="81"/>
+      <c r="F22" s="3">
+        <v>12</v>
+      </c>
+      <c r="G22" s="4">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0.98749999999999993</v>
+      </c>
+      <c r="I22" s="6">
+        <v>0.9902777777777777</v>
+      </c>
+      <c r="J22" s="53">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K22" s="7"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="54" t="str">
+        <v>2.7777777777777679E-3</v>
+      </c>
+      <c r="K22" s="7">
+        <v>3</v>
+      </c>
+      <c r="L22" s="8">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="M22" s="9">
+        <v>12</v>
+      </c>
+      <c r="N22" s="54">
         <f t="shared" si="2"/>
-        <v/>
+        <v>4.8611111111111008E-3</v>
       </c>
       <c r="O22" s="19"/>
       <c r="P22" s="22"/>
@@ -2185,11 +2219,11 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C23" s="77" t="s">
+      <c r="C23" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="77"/>
-      <c r="E23" s="78"/>
+      <c r="D23" s="80"/>
+      <c r="E23" s="81"/>
       <c r="F23" s="3"/>
       <c r="G23" s="4"/>
       <c r="H23" s="5"/>
@@ -2214,20 +2248,40 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C24" s="77" t="s">
+      <c r="C24" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="77"/>
-      <c r="E24" s="78"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="53"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="54"/>
+      <c r="D24" s="80"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="3">
+        <v>10</v>
+      </c>
+      <c r="G24" s="4">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="H24" s="5">
+        <v>0.98125000000000007</v>
+      </c>
+      <c r="I24" s="6">
+        <v>0.98263888888888884</v>
+      </c>
+      <c r="J24" s="53">
+        <f t="shared" si="1"/>
+        <v>1.3888888888887729E-3</v>
+      </c>
+      <c r="K24" s="7">
+        <v>0</v>
+      </c>
+      <c r="L24" s="8">
+        <v>0</v>
+      </c>
+      <c r="M24" s="9">
+        <v>7</v>
+      </c>
+      <c r="N24" s="54">
+        <f t="shared" si="2"/>
+        <v>1.3888888888887729E-3</v>
+      </c>
       <c r="O24" s="19"/>
       <c r="P24" s="22"/>
     </row>
@@ -2237,11 +2291,11 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C25" s="77" t="s">
+      <c r="C25" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="77"/>
-      <c r="E25" s="78"/>
+      <c r="D25" s="80"/>
+      <c r="E25" s="81"/>
       <c r="F25" s="3">
         <v>10</v>
       </c>
@@ -2276,19 +2330,19 @@
     </row>
     <row r="26" spans="1:16" s="27" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="14"/>
-      <c r="B26" s="82" t="s">
+      <c r="B26" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="83"/>
-      <c r="D26" s="83"/>
-      <c r="E26" s="84"/>
+      <c r="C26" s="92"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="93"/>
       <c r="F26" s="45">
         <f>IF(SUM(F18:F25)=0,"Completar",SUM(F18:F25))</f>
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="G26" s="46">
         <f>IF(SUM(G18:G25)=0,"Completar",SUM(G18:G25))</f>
-        <v>2.777777777777778E-2</v>
+        <v>3.4722222222222224E-2</v>
       </c>
       <c r="H26" s="47" t="s">
         <v>32</v>
@@ -2298,23 +2352,23 @@
       </c>
       <c r="J26" s="49">
         <f>IF(OR(COUNTIF(J18:J25,"Error")&gt;0,COUNTIF(J18:J25,"Completar")&gt;0),"Error",IF(SUM(J18:J25)=0,"Completar",SUM(J18:J25)))</f>
-        <v>2.2222222222222476E-2</v>
+        <v>2.6388888888889017E-2</v>
       </c>
       <c r="K26" s="50">
         <f>SUM(K18:K25)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L26" s="46">
         <f>SUM(L18:L25)</f>
-        <v>8.3333333333333332E-3</v>
+        <v>1.0416666666666668E-2</v>
       </c>
       <c r="M26" s="51">
         <f>IF(SUM(M18:M25)=0,"Completar",SUM(M18:M25))</f>
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="N26" s="52">
         <f>IF(OR(COUNTIF(N18:N25,"Error")&gt;0,COUNTIF(N18:N25,"Completar")&gt;0),"Error",IF(SUM(N18:N25)=0,"Completar",SUM(N18:N25)))</f>
-        <v>3.0555555555555808E-2</v>
+        <v>3.6805555555555682E-2</v>
       </c>
       <c r="O26" s="14"/>
       <c r="P26" s="26"/>
@@ -2338,12 +2392,12 @@
     </row>
     <row r="28" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
-      <c r="B28" s="68" t="s">
+      <c r="B28" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="69"/>
-      <c r="D28" s="69"/>
-      <c r="E28" s="70"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="66"/>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
@@ -2420,33 +2474,33 @@
       <c r="O31" s="21"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B32" s="68" t="s">
+      <c r="B32" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="69"/>
-      <c r="D32" s="69"/>
-      <c r="E32" s="69"/>
-      <c r="F32" s="69"/>
-      <c r="G32" s="69"/>
-      <c r="H32" s="69"/>
-      <c r="I32" s="69"/>
-      <c r="J32" s="69"/>
-      <c r="K32" s="69"/>
-      <c r="L32" s="69"/>
-      <c r="M32" s="69"/>
-      <c r="N32" s="70"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="65"/>
+      <c r="I32" s="65"/>
+      <c r="J32" s="65"/>
+      <c r="K32" s="65"/>
+      <c r="L32" s="65"/>
+      <c r="M32" s="65"/>
+      <c r="N32" s="66"/>
     </row>
     <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="79" t="s">
+      <c r="B33" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="80"/>
-      <c r="D33" s="81"/>
-      <c r="E33" s="73">
+      <c r="C33" s="72"/>
+      <c r="D33" s="73"/>
+      <c r="E33" s="82">
         <f>M26</f>
-        <v>86</v>
-      </c>
-      <c r="F33" s="74"/>
+        <v>105</v>
+      </c>
+      <c r="F33" s="83"/>
       <c r="G33" s="29"/>
       <c r="H33" s="30"/>
       <c r="I33" s="30"/>
@@ -2457,16 +2511,16 @@
       <c r="N33" s="31"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B34" s="79" t="s">
+      <c r="B34" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="80"/>
-      <c r="D34" s="81"/>
-      <c r="E34" s="71">
+      <c r="C34" s="72"/>
+      <c r="D34" s="73"/>
+      <c r="E34" s="84">
         <f>IF(M26="Completar","Completar",IFERROR(M26/(N26*24),"Error"))</f>
-        <v>117.2727272727263</v>
-      </c>
-      <c r="F34" s="72"/>
+        <v>118.86792452830147</v>
+      </c>
+      <c r="F34" s="85"/>
       <c r="G34" s="32"/>
       <c r="H34" s="33"/>
       <c r="I34" s="33"/>
@@ -2477,16 +2531,16 @@
       <c r="N34" s="34"/>
     </row>
     <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="79" t="s">
+      <c r="B35" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="80"/>
-      <c r="D35" s="81"/>
-      <c r="E35" s="73">
+      <c r="C35" s="72"/>
+      <c r="D35" s="73"/>
+      <c r="E35" s="82">
         <f>IF(K26=0,0,IFERROR(ROUNDUP(K26/(M26/100),0),"Error"))</f>
-        <v>4</v>
-      </c>
-      <c r="F35" s="74"/>
+        <v>6</v>
+      </c>
+      <c r="F35" s="83"/>
       <c r="G35" s="32"/>
       <c r="H35" s="33"/>
       <c r="I35" s="33"/>
@@ -2497,16 +2551,16 @@
       <c r="N35" s="34"/>
     </row>
     <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="79" t="s">
+      <c r="B36" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="80"/>
-      <c r="D36" s="81"/>
-      <c r="E36" s="85">
+      <c r="C36" s="72"/>
+      <c r="D36" s="73"/>
+      <c r="E36" s="69">
         <f>IF(K26=0,0,IFERROR(K26/M26,"Error"))</f>
-        <v>3.4883720930232558E-2</v>
-      </c>
-      <c r="F36" s="86"/>
+        <v>5.7142857142857141E-2</v>
+      </c>
+      <c r="F36" s="70"/>
       <c r="G36" s="32"/>
       <c r="H36" s="33"/>
       <c r="I36" s="33"/>
@@ -2517,11 +2571,11 @@
       <c r="N36" s="34"/>
     </row>
     <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="79" t="s">
+      <c r="B37" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="80"/>
-      <c r="D37" s="81"/>
+      <c r="C37" s="72"/>
+      <c r="D37" s="73"/>
       <c r="E37" s="57" t="str">
         <f>E5</f>
         <v>Completar</v>
@@ -2540,11 +2594,11 @@
       <c r="N37" s="34"/>
     </row>
     <row r="38" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="79" t="s">
+      <c r="B38" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="80"/>
-      <c r="D38" s="81"/>
+      <c r="C38" s="72"/>
+      <c r="D38" s="73"/>
       <c r="E38" s="57" t="str">
         <f>E9</f>
         <v>Completar</v>
@@ -2563,11 +2617,11 @@
       <c r="N38" s="34"/>
     </row>
     <row r="39" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="79" t="s">
+      <c r="B39" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="C39" s="80"/>
-      <c r="D39" s="81"/>
+      <c r="C39" s="72"/>
+      <c r="D39" s="73"/>
       <c r="E39" s="57" t="str">
         <f>E13</f>
         <v>Completar</v>
@@ -2586,11 +2640,11 @@
       <c r="N39" s="34"/>
     </row>
     <row r="40" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="79" t="s">
+      <c r="B40" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="80"/>
-      <c r="D40" s="81"/>
+      <c r="C40" s="72"/>
+      <c r="D40" s="73"/>
       <c r="E40" s="57" t="str">
         <f>E30</f>
         <v>Completar</v>
@@ -2609,18 +2663,18 @@
       <c r="N40" s="34"/>
     </row>
     <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="79" t="s">
+      <c r="B41" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="80"/>
-      <c r="D41" s="81"/>
+      <c r="C41" s="72"/>
+      <c r="D41" s="73"/>
       <c r="E41" s="57">
         <f>L26</f>
-        <v>8.3333333333333332E-3</v>
+        <v>1.0416666666666668E-2</v>
       </c>
       <c r="F41" s="58">
         <f>IF(E41="Completar",E41,IFERROR(E41/$E$43,"Completar"))</f>
-        <v>0.27272727272727049</v>
+        <v>0.2830188679245273</v>
       </c>
       <c r="G41" s="32"/>
       <c r="H41" s="33"/>
@@ -2632,18 +2686,18 @@
       <c r="N41" s="34"/>
     </row>
     <row r="42" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="79" t="s">
+      <c r="B42" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="C42" s="80"/>
-      <c r="D42" s="81"/>
+      <c r="C42" s="72"/>
+      <c r="D42" s="73"/>
       <c r="E42" s="57">
         <f>J26</f>
-        <v>2.2222222222222476E-2</v>
+        <v>2.6388888888889017E-2</v>
       </c>
       <c r="F42" s="58">
         <f>IF(E42="Completar",E42,IFERROR(E42/$E$43,"Completar"))</f>
-        <v>0.72727272727272962</v>
+        <v>0.71698113207547265</v>
       </c>
       <c r="G42" s="32"/>
       <c r="H42" s="33"/>
@@ -2655,16 +2709,16 @@
       <c r="N42" s="34"/>
     </row>
     <row r="43" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="90" t="s">
+      <c r="B43" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="91"/>
-      <c r="D43" s="92"/>
-      <c r="E43" s="87">
+      <c r="C43" s="78"/>
+      <c r="D43" s="79"/>
+      <c r="E43" s="74">
         <f>IF(COUNTIF(E37:E42,"Error")&gt;0,"Error",IF(SUM(E37:E42)=0,"Completar",SUM(E37:E42)))</f>
-        <v>3.0555555555555808E-2</v>
-      </c>
-      <c r="F43" s="88"/>
+        <v>3.6805555555555688E-2</v>
+      </c>
+      <c r="F43" s="75"/>
       <c r="G43" s="35"/>
       <c r="H43" s="36"/>
       <c r="I43" s="36"/>
@@ -2705,13 +2759,27 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="44">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:N1"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F12:N12"/>
-    <mergeCell ref="F13:N13"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="F8:N8"/>
+    <mergeCell ref="F9:N9"/>
+    <mergeCell ref="B15:N15"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="C16:E17"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="B26:E26"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="B42:D42"/>
     <mergeCell ref="E43:F43"/>
@@ -2728,41 +2796,27 @@
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="B39:D39"/>
     <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="C16:E17"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="F8:N8"/>
-    <mergeCell ref="F9:N9"/>
-    <mergeCell ref="B15:N15"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:N1"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F12:N12"/>
+    <mergeCell ref="F13:N13"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B3:E3"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:B1048576 D1:XFD20 C3:C20 C22:XFD1048576 F21:XFD21">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+  <conditionalFormatting sqref="A1:B1048576 D1:XFD20 C3:C20 F21:XFD21 C22:XFD1048576">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:E21">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>